<commit_message>
uses env variables deploy the application
</commit_message>
<xml_diff>
--- a/test/assets/__modelo.xlsx
+++ b/test/assets/__modelo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\projects\nodejs_mongo_expenses\test\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD3AC95F-6D1D-4071-9735-0D06F13169B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D693065B-6CFC-4457-B08F-6459692BE661}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
   <si>
     <t>Data</t>
   </si>
@@ -73,16 +73,22 @@
     <t>Conta</t>
   </si>
   <si>
-    <t>Conta Inicial</t>
-  </si>
-  <si>
     <t>A definir</t>
+  </si>
+  <si>
+    <t>Conta 1</t>
+  </si>
+  <si>
+    <t>Conta 2</t>
+  </si>
+  <si>
+    <t>Conta 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -583,12 +589,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -601,7 +605,7 @@
     <col min="7" max="16384" width="6.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -621,7 +625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>43328</v>
       </c>
@@ -629,17 +633,17 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3">
         <v>1200</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>43328</v>
       </c>
@@ -654,10 +658,10 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>43328</v>
       </c>
@@ -674,10 +678,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>43329</v>
       </c>
@@ -692,10 +696,10 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>43138</v>
       </c>
@@ -712,10 +716,10 @@
         <v>15</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>43138</v>
       </c>
@@ -732,33 +736,249 @@
         <v>14</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>43328</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="3">
+        <v>1200</v>
+      </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>43328</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>-189.4</v>
+      </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>43328</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3">
+        <v>-94.5</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>43329</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5">
+        <v>-600</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>43138</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-300</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>43138</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-384.5</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>43328</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>43328</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3">
+        <v>-189.4</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>43328</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3">
+        <v>-94.5</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>43329</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5">
+        <v>-600</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>43138</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-300</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>43138</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="3">
+        <v>-384.5</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="2048"/>

</xml_diff>